<commit_message>
solve kriging vsg wrong metrics
</commit_message>
<xml_diff>
--- a/GPR/results_f/all_metrics.xlsx
+++ b/GPR/results_f/all_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,65 +456,45 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>r2_training</t>
+          <t>r2_test</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>mse_training</t>
+          <t>mse_test</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>mape_training</t>
+          <t>mape_test</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>rmse_training</t>
+          <t>rmse_test</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>r2_test</t>
+          <t>r2_vs</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>mse_test</t>
+          <t>mse_vs</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>mape_test</t>
+          <t>mape_vs</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>rmse_test</t>
+          <t>rmse_vs</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>r2_vs</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>mse_vs</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>mape_vs</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_vs</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Kernel</t>
         </is>
@@ -522,54 +502,42 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.7343635241422821</v>
+        <v>0.7343635235672223</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1576932869674099</v>
+        <v>0.1576932873087903</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2322280468477226</v>
+        <v>0.2322280469286339</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3971061406820724</v>
+        <v>0.3971061411119076</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9999999999999986</v>
+        <v>0.9028238131767889</v>
       </c>
       <c r="F2" t="n">
-        <v>1.039892721993923e-15</v>
+        <v>0.08276894642775777</v>
       </c>
       <c r="G2" t="n">
-        <v>1.849132547579974e-08</v>
+        <v>0.2156540326768729</v>
       </c>
       <c r="H2" t="n">
-        <v>3.22473676754231e-08</v>
+        <v>0.2876959270267095</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9028238132913875</v>
+        <v>0.7409829035085965</v>
       </c>
       <c r="J2" t="n">
-        <v>0.08276894633014942</v>
+        <v>0.1618975137598348</v>
       </c>
       <c r="K2" t="n">
-        <v>0.215654032439987</v>
+        <v>0.1896063190244313</v>
       </c>
       <c r="L2" t="n">
-        <v>0.2876959268570715</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.7409829041224776</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.1618975133761312</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.1896063197409963</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.4023649007755661</v>
-      </c>
-      <c r="Q2" t="inlineStr">
+        <v>0.4023649012523767</v>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t>RBF</t>
         </is>
@@ -577,109 +545,85 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.754048321745218</v>
+        <v>0.7540483215612064</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1460075407713272</v>
+        <v>0.1460075408805644</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2489548575541111</v>
+        <v>0.248954857745756</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3821093309137154</v>
+        <v>0.3821093310566551</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.8783149841011321</v>
       </c>
       <c r="F3" t="n">
-        <v>9.126620236270508e-17</v>
+        <v>0.1036441219937698</v>
       </c>
       <c r="G3" t="n">
-        <v>5.68545542969881e-09</v>
+        <v>0.2790110877488802</v>
       </c>
       <c r="H3" t="n">
-        <v>9.553334620053098e-09</v>
+        <v>0.321938071674926</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8783149845908375</v>
+        <v>0.7540739105741914</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1036441215766676</v>
+        <v>0.1537150365209141</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2790110869162588</v>
+        <v>0.2197416489671756</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3219380710271271</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.7540739109098562</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.1537150363111082</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.2197416485544403</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.3920650919313122</v>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Matern_1.5</t>
+        <v>0.3920650921988773</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Matern_0.5</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.7343639066574013</v>
+        <v>0.7343638965567995</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1576930598899114</v>
+        <v>0.157693065886065</v>
       </c>
       <c r="C4" t="n">
-        <v>0.232227985489624</v>
+        <v>0.2322279869070913</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3971058547665992</v>
+        <v>0.3971058623164168</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9999999999999986</v>
+        <v>0.9028239517586609</v>
       </c>
       <c r="F4" t="n">
-        <v>1.039788240372146e-15</v>
+        <v>0.08276882839188993</v>
       </c>
       <c r="G4" t="n">
-        <v>1.849012899218688e-08</v>
+        <v>0.215653964950414</v>
       </c>
       <c r="H4" t="n">
-        <v>3.22457476323956e-08</v>
+        <v>0.2876957218866661</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9028239537580651</v>
+        <v>0.740983340364318</v>
       </c>
       <c r="J4" t="n">
-        <v>0.08276882668891535</v>
+        <v>0.1618972407050592</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2156539608023565</v>
+        <v>0.1896061687584276</v>
       </c>
       <c r="L4" t="n">
-        <v>0.287695718926986</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.7409833511272407</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.161897233977741</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.1896061813107768</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.4023645535801346</v>
-      </c>
-      <c r="Q4" t="inlineStr">
+        <v>0.4023645619398647</v>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>RationalQuadratic</t>
         </is>
@@ -687,54 +631,42 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.7343635166399225</v>
+        <v>0.7343633781643774</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1576932914211347</v>
+        <v>0.1576933736262001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2322280479032267</v>
+        <v>0.2322280673868489</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3971061462897983</v>
+        <v>0.3971062497949385</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9999999999999986</v>
+        <v>0.9028237842013376</v>
       </c>
       <c r="F5" t="n">
-        <v>1.039892318753882e-15</v>
+        <v>0.08276897110733886</v>
       </c>
       <c r="G5" t="n">
-        <v>1.849132448120405e-08</v>
+        <v>0.2156540925739203</v>
       </c>
       <c r="H5" t="n">
-        <v>3.224736142312858e-08</v>
+        <v>0.2876959699184868</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9028238117970018</v>
+        <v>0.7409827482907532</v>
       </c>
       <c r="J5" t="n">
-        <v>0.08276894760297905</v>
+        <v>0.1618976107780753</v>
       </c>
       <c r="K5" t="n">
-        <v>0.2156540355313998</v>
+        <v>0.1896061378365506</v>
       </c>
       <c r="L5" t="n">
-        <v>0.2876959290691807</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.7409828961140774</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.161897518381747</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.1896063103858269</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.4023649069958102</v>
-      </c>
-      <c r="Q5" t="inlineStr">
+        <v>0.4023650218123778</v>
+      </c>
+      <c r="M5" t="inlineStr">
         <is>
           <t>ExpSineSquared</t>
         </is>
@@ -742,54 +674,42 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.03181051529943124</v>
+        <v>-0.03181051529939483</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6125272937751817</v>
+        <v>0.61252729377516</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5797516786088078</v>
+        <v>0.5797516786087576</v>
       </c>
       <c r="D6" t="n">
-        <v>0.782641229284007</v>
+        <v>0.7826412292839932</v>
       </c>
       <c r="E6" t="n">
-        <v>1.068544943461092e-05</v>
+        <v>1.123448542794669e-05</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6974611173260824</v>
+        <v>0.8517314711248334</v>
       </c>
       <c r="G6" t="n">
-        <v>0.54231843148668</v>
+        <v>0.8541377576182823</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8351413756521002</v>
+        <v>0.9228929900724316</v>
       </c>
       <c r="I6" t="n">
-        <v>1.123448555173656e-05</v>
+        <v>-0.0106886765959433</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8517314711247279</v>
+        <v>0.6317265776760479</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8541377576183151</v>
+        <v>0.5357825163404412</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9228929900723745</v>
-      </c>
-      <c r="M6" t="n">
-        <v>-0.01068867659592598</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.6317265776760371</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.5357825163404637</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.7948122908435911</v>
-      </c>
-      <c r="Q6" t="inlineStr">
+        <v>0.7948122908435978</v>
+      </c>
+      <c r="M6" t="inlineStr">
         <is>
           <t>DotProduct</t>
         </is>

</xml_diff>